<commit_message>
Refactor CLM training functions and remove unused code
</commit_message>
<xml_diff>
--- a/valid_unique_smiles_28_02_2025.xlsx
+++ b/valid_unique_smiles_28_02_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Computer\Meh!!!!!!!\workspace\VIT_LAB\SingletFission_ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50AB1588-414F-44D8-9BA5-9E4E59770F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2A18FD-5918-42F1-9BD0-40B5E5F8777A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="889" xr2:uid="{9748B68E-534E-4D07-B84B-E3A578C6F34D}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="889" firstSheet="2" activeTab="4" xr2:uid="{9748B68E-534E-4D07-B84B-E3A578C6F34D}"/>
   </bookViews>
   <sheets>
     <sheet name="valid_unique_smiles_28_02_2025" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="Benzene c1ccccc348" sheetId="3" r:id="rId11"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Polar grp  N+ ( O- )'!$A$1:$C$408</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">valid_unique_smiles_28_02_2025!$A$1:$C$2879</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -19607,8 +19608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4C48EC-BD85-44DC-9405-F7BA30C08339}">
   <dimension ref="A1:C2879"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A8" zoomScale="112" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -53825,15 +53826,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2081DE18-20BE-4B1B-93EE-F628AB19DCC6}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:C408"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="50.6640625" customWidth="1"/>
+    <col min="2" max="2" width="63.44140625" customWidth="1"/>
     <col min="3" max="3" width="78.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -53848,7 +53850,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -53859,7 +53861,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -53870,7 +53872,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -53881,7 +53883,7 @@
         <v>6207</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -53892,7 +53894,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>39</v>
       </c>
@@ -53903,7 +53905,7 @@
         <v>6208</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>59</v>
       </c>
@@ -53925,7 +53927,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>93</v>
       </c>
@@ -53936,7 +53938,7 @@
         <v>6210</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>95</v>
       </c>
@@ -53947,7 +53949,7 @@
         <v>6211</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>103</v>
       </c>
@@ -53969,7 +53971,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>167</v>
       </c>
@@ -53980,7 +53982,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>175</v>
       </c>
@@ -53991,7 +53993,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>205</v>
       </c>
@@ -54002,7 +54004,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>217</v>
       </c>
@@ -54013,7 +54015,7 @@
         <v>6214</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>267</v>
       </c>
@@ -54024,7 +54026,7 @@
         <v>6215</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>273</v>
       </c>
@@ -54035,7 +54037,7 @@
         <v>6216</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>289</v>
       </c>
@@ -54057,7 +54059,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>319</v>
       </c>
@@ -54090,7 +54092,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>367</v>
       </c>
@@ -54123,7 +54125,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>401</v>
       </c>
@@ -54134,7 +54136,7 @@
         <v>6212</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>409</v>
       </c>
@@ -54156,7 +54158,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>429</v>
       </c>
@@ -54167,7 +54169,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>431</v>
       </c>
@@ -54178,7 +54180,7 @@
         <v>6212</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>433</v>
       </c>
@@ -54189,7 +54191,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>447</v>
       </c>
@@ -54200,7 +54202,7 @@
         <v>6207</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>475</v>
       </c>
@@ -54211,7 +54213,7 @@
         <v>6216</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>477</v>
       </c>
@@ -54222,7 +54224,7 @@
         <v>6216</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>495</v>
       </c>
@@ -54233,7 +54235,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>501</v>
       </c>
@@ -54244,7 +54246,7 @@
         <v>6217</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>549</v>
       </c>
@@ -54277,7 +54279,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>601</v>
       </c>
@@ -54299,7 +54301,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>629</v>
       </c>
@@ -54321,7 +54323,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>645</v>
       </c>
@@ -54343,7 +54345,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>683</v>
       </c>
@@ -54354,7 +54356,7 @@
         <v>6207</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>691</v>
       </c>
@@ -54365,7 +54367,7 @@
         <v>6212</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>707</v>
       </c>
@@ -54376,7 +54378,7 @@
         <v>6212</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>709</v>
       </c>
@@ -54398,7 +54400,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>721</v>
       </c>
@@ -54409,7 +54411,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>723</v>
       </c>
@@ -54431,7 +54433,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>751</v>
       </c>
@@ -54442,7 +54444,7 @@
         <v>6216</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>773</v>
       </c>
@@ -54453,7 +54455,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>797</v>
       </c>
@@ -54464,7 +54466,7 @@
         <v>6219</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>829</v>
       </c>
@@ -54486,7 +54488,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>863</v>
       </c>
@@ -54497,7 +54499,7 @@
         <v>6210</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>873</v>
       </c>
@@ -54508,7 +54510,7 @@
         <v>6207</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>905</v>
       </c>
@@ -54519,7 +54521,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>911</v>
       </c>
@@ -54530,7 +54532,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>915</v>
       </c>
@@ -54552,7 +54554,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>927</v>
       </c>
@@ -54563,7 +54565,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>939</v>
       </c>
@@ -54574,7 +54576,7 @@
         <v>6221</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>951</v>
       </c>
@@ -54596,7 +54598,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>957</v>
       </c>
@@ -54618,7 +54620,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>1021</v>
       </c>
@@ -54629,7 +54631,7 @@
         <v>6212</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>1029</v>
       </c>
@@ -54640,7 +54642,7 @@
         <v>6216</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>1047</v>
       </c>
@@ -54651,7 +54653,7 @@
         <v>6208</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>1065</v>
       </c>
@@ -54662,7 +54664,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>1089</v>
       </c>
@@ -54673,7 +54675,7 @@
         <v>6212</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>1091</v>
       </c>
@@ -54684,7 +54686,7 @@
         <v>6193</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>1121</v>
       </c>
@@ -54695,7 +54697,7 @@
         <v>6212</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>1157</v>
       </c>
@@ -54706,7 +54708,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>1161</v>
       </c>
@@ -54717,7 +54719,7 @@
         <v>6207</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>1181</v>
       </c>
@@ -54728,7 +54730,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>1185</v>
       </c>
@@ -54772,7 +54774,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>1223</v>
       </c>
@@ -54783,7 +54785,7 @@
         <v>6207</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>1231</v>
       </c>
@@ -54794,7 +54796,7 @@
         <v>6216</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>1237</v>
       </c>
@@ -54805,7 +54807,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>1337</v>
       </c>
@@ -54816,7 +54818,7 @@
         <v>6223</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>1341</v>
       </c>
@@ -54849,7 +54851,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>1429</v>
       </c>
@@ -54871,7 +54873,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>1445</v>
       </c>
@@ -54882,7 +54884,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>1473</v>
       </c>
@@ -54893,7 +54895,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>1483</v>
       </c>
@@ -54904,7 +54906,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>1495</v>
       </c>
@@ -54915,7 +54917,7 @@
         <v>6207</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>1537</v>
       </c>
@@ -54926,7 +54928,7 @@
         <v>6223</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>1541</v>
       </c>
@@ -54937,7 +54939,7 @@
         <v>6212</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>1555</v>
       </c>
@@ -54948,7 +54950,7 @@
         <v>6224</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>1587</v>
       </c>
@@ -54959,7 +54961,7 @@
         <v>6216</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>1595</v>
       </c>
@@ -54970,7 +54972,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>1599</v>
       </c>
@@ -54981,7 +54983,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>1629</v>
       </c>
@@ -54992,7 +54994,7 @@
         <v>6216</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>1643</v>
       </c>
@@ -55014,7 +55016,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>1653</v>
       </c>
@@ -55025,7 +55027,7 @@
         <v>6212</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>1655</v>
       </c>
@@ -55058,7 +55060,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>1671</v>
       </c>
@@ -55069,7 +55071,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>1673</v>
       </c>
@@ -55080,7 +55082,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>1691</v>
       </c>
@@ -55091,7 +55093,7 @@
         <v>6212</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>1735</v>
       </c>
@@ -55102,7 +55104,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>1739</v>
       </c>
@@ -55113,7 +55115,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>1759</v>
       </c>
@@ -55124,7 +55126,7 @@
         <v>6211</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>1779</v>
       </c>
@@ -55146,7 +55148,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>1801</v>
       </c>
@@ -55168,7 +55170,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>1823</v>
       </c>
@@ -55179,7 +55181,7 @@
         <v>6222</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>1847</v>
       </c>
@@ -55190,7 +55192,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>1855</v>
       </c>
@@ -55201,7 +55203,7 @@
         <v>6216</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>1861</v>
       </c>
@@ -55212,7 +55214,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>1867</v>
       </c>
@@ -55234,7 +55236,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>1875</v>
       </c>
@@ -55245,7 +55247,7 @@
         <v>6212</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>1877</v>
       </c>
@@ -55256,7 +55258,7 @@
         <v>6224</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>1879</v>
       </c>
@@ -55267,7 +55269,7 @@
         <v>6211</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>1885</v>
       </c>
@@ -55311,7 +55313,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>1923</v>
       </c>
@@ -55322,7 +55324,7 @@
         <v>6225</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>1941</v>
       </c>
@@ -55366,7 +55368,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>1977</v>
       </c>
@@ -55388,7 +55390,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>2035</v>
       </c>
@@ -55399,7 +55401,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>2041</v>
       </c>
@@ -55410,7 +55412,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>2053</v>
       </c>
@@ -55421,7 +55423,7 @@
         <v>6227</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>2055</v>
       </c>
@@ -55432,7 +55434,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>2061</v>
       </c>
@@ -55443,7 +55445,7 @@
         <v>6228</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>2067</v>
       </c>
@@ -55454,7 +55456,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>2075</v>
       </c>
@@ -55476,7 +55478,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>2083</v>
       </c>
@@ -55487,7 +55489,7 @@
         <v>6229</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>2091</v>
       </c>
@@ -55509,7 +55511,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>2129</v>
       </c>
@@ -55520,7 +55522,7 @@
         <v>6216</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>2145</v>
       </c>
@@ -55531,7 +55533,7 @@
         <v>6224</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>2147</v>
       </c>
@@ -55553,7 +55555,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>2165</v>
       </c>
@@ -55575,7 +55577,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>2185</v>
       </c>
@@ -55597,7 +55599,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>2199</v>
       </c>
@@ -55608,7 +55610,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>2201</v>
       </c>
@@ -55619,7 +55621,7 @@
         <v>6209</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>2203</v>
       </c>
@@ -55641,7 +55643,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>2215</v>
       </c>
@@ -55652,7 +55654,7 @@
         <v>6226</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>2223</v>
       </c>
@@ -55663,7 +55665,7 @@
         <v>6221</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>2243</v>
       </c>
@@ -55674,7 +55676,7 @@
         <v>6207</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>2259</v>
       </c>
@@ -55707,7 +55709,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>2277</v>
       </c>
@@ -55718,7 +55720,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>2321</v>
       </c>
@@ -55729,7 +55731,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>2335</v>
       </c>
@@ -55740,7 +55742,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>2351</v>
       </c>
@@ -55762,7 +55764,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>2377</v>
       </c>
@@ -55773,7 +55775,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>2391</v>
       </c>
@@ -55784,7 +55786,7 @@
         <v>6230</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>2413</v>
       </c>
@@ -55795,7 +55797,7 @@
         <v>6209</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>2443</v>
       </c>
@@ -55806,7 +55808,7 @@
         <v>6231</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>2457</v>
       </c>
@@ -55817,7 +55819,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>2487</v>
       </c>
@@ -55850,7 +55852,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>2563</v>
       </c>
@@ -55861,7 +55863,7 @@
         <v>6229</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>2565</v>
       </c>
@@ -55872,7 +55874,7 @@
         <v>6223</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>2567</v>
       </c>
@@ -55883,7 +55885,7 @@
         <v>6229</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>2573</v>
       </c>
@@ -55894,7 +55896,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>2583</v>
       </c>
@@ -55905,7 +55907,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
         <v>2645</v>
       </c>
@@ -55916,7 +55918,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>2653</v>
       </c>
@@ -55938,7 +55940,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>2661</v>
       </c>
@@ -55949,7 +55951,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
         <v>2679</v>
       </c>
@@ -55982,7 +55984,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>2739</v>
       </c>
@@ -55993,7 +55995,7 @@
         <v>6207</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
         <v>2795</v>
       </c>
@@ -56037,7 +56039,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
         <v>2871</v>
       </c>
@@ -56048,7 +56050,7 @@
         <v>6212</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
         <v>2907</v>
       </c>
@@ -56059,7 +56061,7 @@
         <v>6209</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
         <v>2943</v>
       </c>
@@ -56070,7 +56072,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
         <v>2947</v>
       </c>
@@ -56081,7 +56083,7 @@
         <v>6209</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
         <v>2953</v>
       </c>
@@ -56114,7 +56116,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>3027</v>
       </c>
@@ -56147,7 +56149,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
         <v>3039</v>
       </c>
@@ -56169,7 +56171,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
         <v>3061</v>
       </c>
@@ -56180,7 +56182,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
         <v>3071</v>
       </c>
@@ -56191,7 +56193,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
         <v>3073</v>
       </c>
@@ -56213,7 +56215,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
         <v>3133</v>
       </c>
@@ -56235,7 +56237,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
         <v>3149</v>
       </c>
@@ -56257,7 +56259,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
         <v>3231</v>
       </c>
@@ -56268,7 +56270,7 @@
         <v>6223</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
         <v>3237</v>
       </c>
@@ -56279,7 +56281,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
         <v>3257</v>
       </c>
@@ -56301,7 +56303,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
         <v>3267</v>
       </c>
@@ -56312,7 +56314,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>3273</v>
       </c>
@@ -56323,7 +56325,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
         <v>3281</v>
       </c>
@@ -56334,7 +56336,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
         <v>3285</v>
       </c>
@@ -56345,7 +56347,7 @@
         <v>6184</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
         <v>3287</v>
       </c>
@@ -56356,7 +56358,7 @@
         <v>6211</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
         <v>3295</v>
       </c>
@@ -56378,7 +56380,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
         <v>3307</v>
       </c>
@@ -56389,7 +56391,7 @@
         <v>6212</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" s="1" t="s">
         <v>3323</v>
       </c>
@@ -56400,7 +56402,7 @@
         <v>6222</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
         <v>3327</v>
       </c>
@@ -56411,7 +56413,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" s="1" t="s">
         <v>3337</v>
       </c>
@@ -56422,7 +56424,7 @@
         <v>6226</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" s="1" t="s">
         <v>3339</v>
       </c>
@@ -56433,7 +56435,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237" s="1" t="s">
         <v>3351</v>
       </c>
@@ -56444,7 +56446,7 @@
         <v>6233</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
         <v>3369</v>
       </c>
@@ -56455,7 +56457,7 @@
         <v>6232</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239" s="1" t="s">
         <v>3375</v>
       </c>
@@ -56466,7 +56468,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A240" s="1" t="s">
         <v>3379</v>
       </c>
@@ -56488,7 +56490,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
         <v>3419</v>
       </c>
@@ -56510,7 +56512,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244" s="1" t="s">
         <v>3453</v>
       </c>
@@ -56532,7 +56534,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246" s="1" t="s">
         <v>3473</v>
       </c>
@@ -56554,7 +56556,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" s="1" t="s">
         <v>3501</v>
       </c>
@@ -56565,7 +56567,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249" s="1" t="s">
         <v>3513</v>
       </c>
@@ -56576,7 +56578,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
         <v>3515</v>
       </c>
@@ -56587,7 +56589,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251" s="1" t="s">
         <v>3541</v>
       </c>
@@ -56620,7 +56622,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" s="1" t="s">
         <v>3567</v>
       </c>
@@ -56631,7 +56633,7 @@
         <v>6212</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
         <v>3585</v>
       </c>
@@ -56642,7 +56644,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
         <v>3603</v>
       </c>
@@ -56653,7 +56655,7 @@
         <v>6216</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257" s="1" t="s">
         <v>3641</v>
       </c>
@@ -56675,7 +56677,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259" s="1" t="s">
         <v>3655</v>
       </c>
@@ -56686,7 +56688,7 @@
         <v>6224</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260" s="1" t="s">
         <v>3701</v>
       </c>
@@ -56708,7 +56710,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262" s="1" t="s">
         <v>3731</v>
       </c>
@@ -56741,7 +56743,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265" s="1" t="s">
         <v>3787</v>
       </c>
@@ -56774,7 +56776,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268" s="1" t="s">
         <v>3873</v>
       </c>
@@ -56807,7 +56809,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271" s="1" t="s">
         <v>3923</v>
       </c>
@@ -56818,7 +56820,7 @@
         <v>6212</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272" s="1" t="s">
         <v>3927</v>
       </c>
@@ -56829,7 +56831,7 @@
         <v>6207</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A273" s="1" t="s">
         <v>3931</v>
       </c>
@@ -56840,7 +56842,7 @@
         <v>6221</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A274" s="1" t="s">
         <v>3935</v>
       </c>
@@ -56862,7 +56864,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A276" s="1" t="s">
         <v>3951</v>
       </c>
@@ -56884,7 +56886,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A278" s="1" t="s">
         <v>3959</v>
       </c>
@@ -56895,7 +56897,7 @@
         <v>6234</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279" s="1" t="s">
         <v>3963</v>
       </c>
@@ -56917,7 +56919,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A281" s="1" t="s">
         <v>4029</v>
       </c>
@@ -56928,7 +56930,7 @@
         <v>6210</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A282" s="1" t="s">
         <v>4059</v>
       </c>
@@ -56950,7 +56952,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A284" s="1" t="s">
         <v>4089</v>
       </c>
@@ -56961,7 +56963,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A285" s="1" t="s">
         <v>4095</v>
       </c>
@@ -56972,7 +56974,7 @@
         <v>6216</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A286" s="1" t="s">
         <v>4103</v>
       </c>
@@ -56983,7 +56985,7 @@
         <v>6226</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A287" s="1" t="s">
         <v>4111</v>
       </c>
@@ -56994,7 +56996,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A288" s="1" t="s">
         <v>4115</v>
       </c>
@@ -57005,7 +57007,7 @@
         <v>6225</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A289" s="1" t="s">
         <v>4131</v>
       </c>
@@ -57016,7 +57018,7 @@
         <v>6216</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A290" s="1" t="s">
         <v>4139</v>
       </c>
@@ -57027,7 +57029,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291" s="1" t="s">
         <v>4141</v>
       </c>
@@ -57038,7 +57040,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A292" s="1" t="s">
         <v>4151</v>
       </c>
@@ -57060,7 +57062,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A294" s="1" t="s">
         <v>4159</v>
       </c>
@@ -57071,7 +57073,7 @@
         <v>6212</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A295" s="1" t="s">
         <v>4163</v>
       </c>
@@ -57082,7 +57084,7 @@
         <v>6209</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A296" s="1" t="s">
         <v>4167</v>
       </c>
@@ -57104,7 +57106,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A298" s="1" t="s">
         <v>4191</v>
       </c>
@@ -57126,7 +57128,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300" s="1" t="s">
         <v>4213</v>
       </c>
@@ -57137,7 +57139,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A301" s="1" t="s">
         <v>4287</v>
       </c>
@@ -57148,7 +57150,7 @@
         <v>6224</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A302" s="1" t="s">
         <v>4289</v>
       </c>
@@ -57170,7 +57172,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A304" s="1" t="s">
         <v>4333</v>
       </c>
@@ -57181,7 +57183,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A305" s="1" t="s">
         <v>4335</v>
       </c>
@@ -57192,7 +57194,7 @@
         <v>6207</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A306" s="1" t="s">
         <v>4357</v>
       </c>
@@ -57203,7 +57205,7 @@
         <v>6229</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A307" s="1" t="s">
         <v>4363</v>
       </c>
@@ -57214,7 +57216,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A308" s="1" t="s">
         <v>4373</v>
       </c>
@@ -57247,7 +57249,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A311" s="1" t="s">
         <v>4425</v>
       </c>
@@ -57258,7 +57260,7 @@
         <v>6223</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A312" s="1" t="s">
         <v>4447</v>
       </c>
@@ -57269,7 +57271,7 @@
         <v>6223</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A313" s="1" t="s">
         <v>4453</v>
       </c>
@@ -57280,7 +57282,7 @@
         <v>6236</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A314" s="1" t="s">
         <v>4469</v>
       </c>
@@ -57291,7 +57293,7 @@
         <v>6221</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A315" s="1" t="s">
         <v>4475</v>
       </c>
@@ -57302,7 +57304,7 @@
         <v>6218</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A316" s="1" t="s">
         <v>4479</v>
       </c>
@@ -57313,7 +57315,7 @@
         <v>6223</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A317" s="1" t="s">
         <v>4481</v>
       </c>
@@ -57324,7 +57326,7 @@
         <v>6210</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A318" s="1" t="s">
         <v>4517</v>
       </c>
@@ -57335,7 +57337,7 @@
         <v>6212</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A319" s="1" t="s">
         <v>4525</v>
       </c>
@@ -57346,7 +57348,7 @@
         <v>6216</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A320" s="1" t="s">
         <v>4557</v>
       </c>
@@ -57368,7 +57370,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A322" s="1" t="s">
         <v>4603</v>
       </c>
@@ -57379,7 +57381,7 @@
         <v>6212</v>
       </c>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A323" s="1" t="s">
         <v>4607</v>
       </c>
@@ -57390,7 +57392,7 @@
         <v>6209</v>
       </c>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A324" s="1" t="s">
         <v>4617</v>
       </c>
@@ -57412,7 +57414,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A326" s="1" t="s">
         <v>4653</v>
       </c>
@@ -57423,7 +57425,7 @@
         <v>6228</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A327" s="1" t="s">
         <v>4673</v>
       </c>
@@ -57434,7 +57436,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A328" s="1" t="s">
         <v>4677</v>
       </c>
@@ -57456,7 +57458,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A330" s="1" t="s">
         <v>4693</v>
       </c>
@@ -57467,7 +57469,7 @@
         <v>6223</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A331" s="1" t="s">
         <v>4729</v>
       </c>
@@ -57478,7 +57480,7 @@
         <v>6211</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A332" s="1" t="s">
         <v>4739</v>
       </c>
@@ -57489,7 +57491,7 @@
         <v>6232</v>
       </c>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A333" s="1" t="s">
         <v>4767</v>
       </c>
@@ -57511,7 +57513,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A335" s="1" t="s">
         <v>4795</v>
       </c>
@@ -57522,7 +57524,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A336" s="1" t="s">
         <v>4797</v>
       </c>
@@ -57544,7 +57546,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A338" s="1" t="s">
         <v>4809</v>
       </c>
@@ -57555,7 +57557,7 @@
         <v>6216</v>
       </c>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A339" s="1" t="s">
         <v>4861</v>
       </c>
@@ -57566,7 +57568,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A340" s="1" t="s">
         <v>4869</v>
       </c>
@@ -57610,7 +57612,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A344" s="1" t="s">
         <v>4909</v>
       </c>
@@ -57643,7 +57645,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A347" s="1" t="s">
         <v>4927</v>
       </c>
@@ -57654,7 +57656,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A348" s="1" t="s">
         <v>4941</v>
       </c>
@@ -57665,7 +57667,7 @@
         <v>6216</v>
       </c>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A349" s="1" t="s">
         <v>4947</v>
       </c>
@@ -57676,7 +57678,7 @@
         <v>6222</v>
       </c>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A350" s="1" t="s">
         <v>4949</v>
       </c>
@@ -57687,7 +57689,7 @@
         <v>6226</v>
       </c>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A351" s="1" t="s">
         <v>4965</v>
       </c>
@@ -57698,7 +57700,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A352" s="1" t="s">
         <v>5007</v>
       </c>
@@ -57709,7 +57711,7 @@
         <v>6224</v>
       </c>
     </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A353" s="1" t="s">
         <v>5015</v>
       </c>
@@ -57720,7 +57722,7 @@
         <v>6235</v>
       </c>
     </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A354" s="1" t="s">
         <v>5033</v>
       </c>
@@ -57731,7 +57733,7 @@
         <v>6229</v>
       </c>
     </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A355" s="1" t="s">
         <v>5041</v>
       </c>
@@ -57742,7 +57744,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A356" s="1" t="s">
         <v>5051</v>
       </c>
@@ -57753,7 +57755,7 @@
         <v>6212</v>
       </c>
     </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A357" s="1" t="s">
         <v>5061</v>
       </c>
@@ -57764,7 +57766,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A358" s="1" t="s">
         <v>5063</v>
       </c>
@@ -57775,7 +57777,7 @@
         <v>6237</v>
       </c>
     </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A359" s="1" t="s">
         <v>5067</v>
       </c>
@@ -57786,7 +57788,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A360" s="1" t="s">
         <v>5107</v>
       </c>
@@ -57797,7 +57799,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A361" s="1" t="s">
         <v>5113</v>
       </c>
@@ -57808,7 +57810,7 @@
         <v>6216</v>
       </c>
     </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A362" s="1" t="s">
         <v>5115</v>
       </c>
@@ -57841,7 +57843,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A365" s="1" t="s">
         <v>5167</v>
       </c>
@@ -57852,7 +57854,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A366" s="1" t="s">
         <v>5191</v>
       </c>
@@ -57874,7 +57876,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A368" s="1" t="s">
         <v>5209</v>
       </c>
@@ -57907,7 +57909,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A371" s="1" t="s">
         <v>5233</v>
       </c>
@@ -57918,7 +57920,7 @@
         <v>6210</v>
       </c>
     </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A372" s="1" t="s">
         <v>5239</v>
       </c>
@@ -57940,7 +57942,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A374" s="1" t="s">
         <v>5267</v>
       </c>
@@ -57951,7 +57953,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A375" s="1" t="s">
         <v>5269</v>
       </c>
@@ -57973,7 +57975,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A377" s="1" t="s">
         <v>5295</v>
       </c>
@@ -57995,7 +57997,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A379" s="1" t="s">
         <v>5319</v>
       </c>
@@ -58006,7 +58008,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A380" s="1" t="s">
         <v>5323</v>
       </c>
@@ -58039,7 +58041,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A383" s="1" t="s">
         <v>5355</v>
       </c>
@@ -58050,7 +58052,7 @@
         <v>6207</v>
       </c>
     </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A384" s="1" t="s">
         <v>5359</v>
       </c>
@@ -58072,7 +58074,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="386" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A386" s="1" t="s">
         <v>5367</v>
       </c>
@@ -58083,7 +58085,7 @@
         <v>6216</v>
       </c>
     </row>
-    <row r="387" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A387" s="1" t="s">
         <v>5395</v>
       </c>
@@ -58094,7 +58096,7 @@
         <v>6224</v>
       </c>
     </row>
-    <row r="388" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A388" s="1" t="s">
         <v>5405</v>
       </c>
@@ -58105,7 +58107,7 @@
         <v>6207</v>
       </c>
     </row>
-    <row r="389" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A389" s="1" t="s">
         <v>5439</v>
       </c>
@@ -58116,7 +58118,7 @@
         <v>6213</v>
       </c>
     </row>
-    <row r="390" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A390" s="1" t="s">
         <v>5443</v>
       </c>
@@ -58138,7 +58140,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="392" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A392" s="1" t="s">
         <v>5477</v>
       </c>
@@ -58149,7 +58151,7 @@
         <v>6223</v>
       </c>
     </row>
-    <row r="393" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A393" s="1" t="s">
         <v>5481</v>
       </c>
@@ -58160,7 +58162,7 @@
         <v>6212</v>
       </c>
     </row>
-    <row r="394" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A394" s="1" t="s">
         <v>5519</v>
       </c>
@@ -58171,7 +58173,7 @@
         <v>6226</v>
       </c>
     </row>
-    <row r="395" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A395" s="1" t="s">
         <v>5537</v>
       </c>
@@ -58182,7 +58184,7 @@
         <v>6232</v>
       </c>
     </row>
-    <row r="396" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A396" s="1" t="s">
         <v>5555</v>
       </c>
@@ -58193,7 +58195,7 @@
         <v>6216</v>
       </c>
     </row>
-    <row r="397" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A397" s="1" t="s">
         <v>5561</v>
       </c>
@@ -58204,7 +58206,7 @@
         <v>6238</v>
       </c>
     </row>
-    <row r="398" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A398" s="1" t="s">
         <v>5575</v>
       </c>
@@ -58215,7 +58217,7 @@
         <v>6211</v>
       </c>
     </row>
-    <row r="399" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A399" s="1" t="s">
         <v>5583</v>
       </c>
@@ -58226,7 +58228,7 @@
         <v>6231</v>
       </c>
     </row>
-    <row r="400" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A400" s="1" t="s">
         <v>5585</v>
       </c>
@@ -58237,7 +58239,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="401" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A401" s="1" t="s">
         <v>5601</v>
       </c>
@@ -58248,7 +58250,7 @@
         <v>6209</v>
       </c>
     </row>
-    <row r="402" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A402" s="1" t="s">
         <v>5623</v>
       </c>
@@ -58259,7 +58261,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="403" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A403" s="1" t="s">
         <v>5649</v>
       </c>
@@ -58270,7 +58272,7 @@
         <v>6232</v>
       </c>
     </row>
-    <row r="404" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A404" s="1" t="s">
         <v>5651</v>
       </c>
@@ -58281,7 +58283,7 @@
         <v>6231</v>
       </c>
     </row>
-    <row r="405" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A405" s="1" t="s">
         <v>5681</v>
       </c>
@@ -58292,7 +58294,7 @@
         <v>6223</v>
       </c>
     </row>
-    <row r="406" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A406" s="1" t="s">
         <v>5687</v>
       </c>
@@ -58303,7 +58305,7 @@
         <v>6227</v>
       </c>
     </row>
-    <row r="407" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A407" s="1" t="s">
         <v>5713</v>
       </c>
@@ -58314,7 +58316,7 @@
         <v>6229</v>
       </c>
     </row>
-    <row r="408" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A408" s="1" t="s">
         <v>5721</v>
       </c>
@@ -58326,6 +58328,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C408" xr:uid="{2081DE18-20BE-4B1B-93EE-F628AB19DCC6}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Polar grp: [N+]([O-])"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -58334,8 +58343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF863F8-6C85-4B85-BCBA-F028D2702A82}">
   <dimension ref="A1:C283"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -61466,8 +61475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9E3F1DE-31E7-496E-9B31-FBEF5B5E89C8}">
   <dimension ref="A1:C567"/>
   <sheetViews>
-    <sheetView topLeftCell="A541" workbookViewId="0">
-      <selection activeCell="C567" sqref="C567"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -67722,8 +67731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0753FDE-2704-42A7-8B27-0CDB8EEB4622}">
   <dimension ref="A1:C226"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Remove Book1.xlsx and add Used_SMILES.xlsx with updated data
</commit_message>
<xml_diff>
--- a/valid_unique_smiles_28_02_2025.xlsx
+++ b/valid_unique_smiles_28_02_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Computer\Meh!!!!!!!\workspace\VIT_LAB\SingletFission_ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2A18FD-5918-42F1-9BD0-40B5E5F8777A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301634E2-8FEB-4B7B-A23F-D68A7027A581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="889" firstSheet="2" activeTab="4" xr2:uid="{9748B68E-534E-4D07-B84B-E3A578C6F34D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="889" activeTab="7" xr2:uid="{9748B68E-534E-4D07-B84B-E3A578C6F34D}"/>
   </bookViews>
   <sheets>
     <sheet name="valid_unique_smiles_28_02_2025" sheetId="1" r:id="rId1"/>
@@ -18902,7 +18902,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -19082,6 +19082,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -19243,7 +19249,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -19251,6 +19257,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -53830,7 +53840,7 @@
   <dimension ref="A1:C408"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A26" sqref="A26:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -54115,13 +54125,13 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="3" t="s">
         <v>6205</v>
       </c>
     </row>
@@ -58343,8 +58353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF863F8-6C85-4B85-BCBA-F028D2702A82}">
   <dimension ref="A1:C283"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -58486,13 +58496,13 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="3" t="s">
         <v>6190</v>
       </c>
     </row>
@@ -61476,7 +61486,7 @@
   <dimension ref="A1:C567"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -67731,8 +67741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0753FDE-2704-42A7-8B27-0CDB8EEB4622}">
   <dimension ref="A1:C226"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -67830,13 +67840,13 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>6161</v>
       </c>
     </row>
@@ -70236,8 +70246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DB8260-6AF3-401C-924C-60795708A8D7}">
   <dimension ref="A1:C861"/>
   <sheetViews>
-    <sheetView topLeftCell="A835" workbookViewId="0">
-      <selection activeCell="C861" sqref="C861"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -70423,13 +70433,13 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="3" t="s">
         <v>6151</v>
       </c>
     </row>
@@ -79727,7 +79737,7 @@
   <dimension ref="A1:C89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A8" sqref="A8:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -79814,13 +79824,13 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>447</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>448</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>6141</v>
       </c>
     </row>
@@ -80724,8 +80734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B24ED4DC-C2C5-4EA6-83FE-054DAE2A54A1}">
   <dimension ref="A1:C476"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -80911,13 +80921,13 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="3" t="s">
         <v>6134</v>
       </c>
     </row>
@@ -85980,7 +85990,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -86078,13 +86088,13 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>4221</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>4222</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>6131</v>
       </c>
     </row>

</xml_diff>